<commit_message>
updated the bar chart
</commit_message>
<xml_diff>
--- a/public/assets/data/Business License.xlsx
+++ b/public/assets/data/Business License.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Web Dev\React\tax-system\public\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A31158-0E4A-42B7-A5E9-56A892C47DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F94E06-F630-4869-BEE1-458D2B73C770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{8E89FA64-FD5D-7044-A3F7-FA21A61CA12E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8E89FA64-FD5D-7044-A3F7-FA21A61CA12E}"/>
   </bookViews>
   <sheets>
     <sheet name="License" sheetId="1" r:id="rId1"/>
@@ -1145,21 +1145,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1168,6 +1153,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1485,8 +1485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB7BB918-6CF2-C84C-BA02-622A62B1D029}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="B44" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1523,10 +1523,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="40">
+      <c r="A2" s="41">
         <v>1</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="41" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1540,16 +1540,16 @@
       </c>
       <c r="F2" s="6">
         <f ca="1">RANDBETWEEN(100000,350000)</f>
-        <v>296487</v>
-      </c>
-      <c r="G2" s="39">
+        <v>124311</v>
+      </c>
+      <c r="G2" s="44">
         <f ca="1">F2+F3+F4</f>
-        <v>656574</v>
+        <v>780233</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
@@ -1558,17 +1558,17 @@
       </c>
       <c r="E3" s="3">
         <f ca="1">RANDBETWEEN(10,50)</f>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F3" s="6">
         <f t="shared" ref="F3:F61" ca="1" si="0">RANDBETWEEN(100000,350000)</f>
-        <v>116867</v>
-      </c>
-      <c r="G3" s="39"/>
+        <v>349839</v>
+      </c>
+      <c r="G3" s="44"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="4" t="s">
         <v>25</v>
       </c>
@@ -1577,19 +1577,19 @@
       </c>
       <c r="E4" s="3">
         <f t="shared" ref="E4:E61" ca="1" si="1">RANDBETWEEN(10,50)</f>
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="F4" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>243220</v>
-      </c>
-      <c r="G4" s="39"/>
+        <v>306083</v>
+      </c>
+      <c r="G4" s="44"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="40">
+      <c r="A5" s="41">
         <v>2</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="41" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1597,66 +1597,66 @@
       </c>
       <c r="D5" s="3">
         <f ca="1">RANDBETWEEN(80,300)</f>
-        <v>292</v>
+        <v>200</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>344623</v>
-      </c>
-      <c r="G5" s="39">
+        <v>202497</v>
+      </c>
+      <c r="G5" s="44">
         <f t="shared" ref="G5" ca="1" si="2">F5+F6+F7</f>
-        <v>804456</v>
+        <v>708532</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ref="D6:D61" ca="1" si="3">RANDBETWEEN(80,300)</f>
-        <v>296</v>
+        <v>237</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>139331</v>
-      </c>
-      <c r="G6" s="39"/>
+        <v>163009</v>
+      </c>
+      <c r="G6" s="44"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="40"/>
-      <c r="B7" s="40"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>290</v>
+        <v>263</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="F7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>320502</v>
-      </c>
-      <c r="G7" s="39"/>
+        <v>343026</v>
+      </c>
+      <c r="G7" s="44"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="40">
+      <c r="A8" s="41">
         <v>3</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="41" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1664,66 +1664,66 @@
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>290101</v>
-      </c>
-      <c r="G8" s="39">
+        <v>155216</v>
+      </c>
+      <c r="G8" s="44">
         <f t="shared" ref="G8" ca="1" si="4">F8+F9+F10</f>
-        <v>803537</v>
+        <v>826256</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>270</v>
+        <v>116</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="F9" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>180750</v>
-      </c>
-      <c r="G9" s="39"/>
+        <v>331882</v>
+      </c>
+      <c r="G9" s="44"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>106</v>
+        <v>229</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F10" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>332686</v>
-      </c>
-      <c r="G10" s="39"/>
+        <v>339158</v>
+      </c>
+      <c r="G10" s="44"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="40">
+      <c r="A11" s="41">
         <v>4</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1731,66 +1731,66 @@
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F11" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>218893</v>
-      </c>
-      <c r="G11" s="39">
+        <v>345710</v>
+      </c>
+      <c r="G11" s="44">
         <f t="shared" ref="G11" ca="1" si="5">F11+F12+F13</f>
-        <v>800522</v>
+        <v>655430</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="40"/>
-      <c r="B12" s="40"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>82</v>
+        <v>192</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F12" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>297655</v>
-      </c>
-      <c r="G12" s="39"/>
+        <v>150814</v>
+      </c>
+      <c r="G12" s="44"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="40"/>
-      <c r="B13" s="40"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="41"/>
       <c r="C13" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>228</v>
+        <v>202</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F13" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>283974</v>
-      </c>
-      <c r="G13" s="39"/>
+        <v>158906</v>
+      </c>
+      <c r="G13" s="44"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="40">
+      <c r="A14" s="41">
         <v>5</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="41" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1798,66 +1798,66 @@
       </c>
       <c r="D14" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>267</v>
+        <v>222</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="F14" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>250007</v>
-      </c>
-      <c r="G14" s="39">
+        <v>231926</v>
+      </c>
+      <c r="G14" s="44">
         <f t="shared" ref="G14" ca="1" si="6">F14+F15+F16</f>
-        <v>652747</v>
+        <v>606654</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>240</v>
+        <v>292</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F15" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>184235</v>
-      </c>
-      <c r="G15" s="39"/>
+        <v>213526</v>
+      </c>
+      <c r="G15" s="44"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>145</v>
+        <v>238</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="F16" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>218505</v>
-      </c>
-      <c r="G16" s="39"/>
+        <v>161202</v>
+      </c>
+      <c r="G16" s="44"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="40">
+      <c r="A17" s="41">
         <v>6</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="41" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -1865,7 +1865,7 @@
       </c>
       <c r="D17" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>219</v>
+        <v>300</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" ca="1" si="1"/>
@@ -1873,58 +1873,58 @@
       </c>
       <c r="F17" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>121069</v>
-      </c>
-      <c r="G17" s="39">
+        <v>179952</v>
+      </c>
+      <c r="G17" s="44">
         <f t="shared" ref="G17" ca="1" si="7">F17+F18+F19</f>
-        <v>708654</v>
+        <v>622293</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>250</v>
+        <v>112</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="F18" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>339441</v>
-      </c>
-      <c r="G18" s="39"/>
+        <v>140408</v>
+      </c>
+      <c r="G18" s="44"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D19" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>218</v>
+        <v>82</v>
       </c>
       <c r="E19" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F19" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>248144</v>
-      </c>
-      <c r="G19" s="39"/>
+        <v>301933</v>
+      </c>
+      <c r="G19" s="44"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="40">
+      <c r="A20" s="41">
         <v>7</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="41" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -1932,66 +1932,66 @@
       </c>
       <c r="D20" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E20" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="F20" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>260006</v>
-      </c>
-      <c r="G20" s="39">
+        <v>104639</v>
+      </c>
+      <c r="G20" s="44">
         <f t="shared" ref="G20" ca="1" si="8">F20+F21+F22</f>
-        <v>794305</v>
+        <v>499769</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="40"/>
-      <c r="B21" s="40"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>174</v>
+        <v>276</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F21" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>290621</v>
-      </c>
-      <c r="G21" s="39"/>
+        <v>236324</v>
+      </c>
+      <c r="G21" s="44"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="40"/>
-      <c r="B22" s="40"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D22" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>298</v>
+        <v>193</v>
       </c>
       <c r="E22" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="F22" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>243678</v>
-      </c>
-      <c r="G22" s="39"/>
+        <v>158806</v>
+      </c>
+      <c r="G22" s="44"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="40">
+      <c r="A23" s="41">
         <v>8</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="41" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1999,66 +1999,66 @@
       </c>
       <c r="D23" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="E23" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F23" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>165982</v>
-      </c>
-      <c r="G23" s="39">
+        <v>293536</v>
+      </c>
+      <c r="G23" s="44">
         <f t="shared" ref="G23" ca="1" si="9">F23+F24+F25</f>
-        <v>568198</v>
+        <v>954308</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="E24" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F24" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>144677</v>
-      </c>
-      <c r="G24" s="39"/>
+        <v>314994</v>
+      </c>
+      <c r="G24" s="44"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="40"/>
-      <c r="B25" s="40"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
       <c r="C25" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D25" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>234</v>
+        <v>295</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="F25" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>257539</v>
-      </c>
-      <c r="G25" s="39"/>
+        <v>345778</v>
+      </c>
+      <c r="G25" s="44"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="40">
+      <c r="A26" s="41">
         <v>9</v>
       </c>
-      <c r="B26" s="41" t="s">
+      <c r="B26" s="43" t="s">
         <v>10</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -2066,66 +2066,66 @@
       </c>
       <c r="D26" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>213</v>
+        <v>87</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F26" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>176182</v>
-      </c>
-      <c r="G26" s="39">
+        <v>240891</v>
+      </c>
+      <c r="G26" s="44">
         <f t="shared" ref="G26" ca="1" si="10">F26+F27+F28</f>
-        <v>619591</v>
+        <v>831159</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="40"/>
-      <c r="B27" s="41"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="43"/>
       <c r="C27" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>216</v>
+        <v>180</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F27" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>275492</v>
-      </c>
-      <c r="G27" s="39"/>
+        <v>249487</v>
+      </c>
+      <c r="G27" s="44"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="40"/>
-      <c r="B28" s="41"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="43"/>
       <c r="C28" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D28" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>224</v>
+        <v>102</v>
       </c>
       <c r="E28" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="F28" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>167917</v>
-      </c>
-      <c r="G28" s="39"/>
+        <v>340781</v>
+      </c>
+      <c r="G28" s="44"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="40">
+      <c r="A29" s="41">
         <v>10</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="41" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -2133,66 +2133,66 @@
       </c>
       <c r="D29" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>291</v>
+        <v>231</v>
       </c>
       <c r="E29" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="F29" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>214053</v>
-      </c>
-      <c r="G29" s="39">
+        <v>255716</v>
+      </c>
+      <c r="G29" s="44">
         <f t="shared" ref="G29" ca="1" si="11">F29+F30+F31</f>
-        <v>834650</v>
+        <v>583397</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="40"/>
-      <c r="B30" s="40"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="E30" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="F30" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>327148</v>
-      </c>
-      <c r="G30" s="39"/>
+        <v>112099</v>
+      </c>
+      <c r="G30" s="44"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="40"/>
-      <c r="B31" s="40"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D31" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>185</v>
+        <v>299</v>
       </c>
       <c r="E31" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F31" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>293449</v>
-      </c>
-      <c r="G31" s="39"/>
+        <v>215582</v>
+      </c>
+      <c r="G31" s="44"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="40">
+      <c r="A32" s="41">
         <v>11</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="41" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -2200,66 +2200,66 @@
       </c>
       <c r="D32" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>156</v>
+        <v>284</v>
       </c>
       <c r="E32" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="F32" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>242323</v>
-      </c>
-      <c r="G32" s="39">
+        <v>202911</v>
+      </c>
+      <c r="G32" s="44">
         <f t="shared" ref="G32" ca="1" si="12">F32+F33+F34</f>
-        <v>870810</v>
+        <v>627090</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="40"/>
-      <c r="B33" s="40"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="41"/>
       <c r="C33" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D33" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="E33" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="F33" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>342136</v>
-      </c>
-      <c r="G33" s="39"/>
+        <v>321933</v>
+      </c>
+      <c r="G33" s="44"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="40"/>
-      <c r="B34" s="40"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="41"/>
       <c r="C34" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D34" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="E34" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F34" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>286351</v>
-      </c>
-      <c r="G34" s="39"/>
+        <v>102246</v>
+      </c>
+      <c r="G34" s="44"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="40">
+      <c r="A35" s="41">
         <v>12</v>
       </c>
-      <c r="B35" s="40" t="s">
+      <c r="B35" s="41" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -2267,66 +2267,66 @@
       </c>
       <c r="D35" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>195</v>
+        <v>284</v>
       </c>
       <c r="E35" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="F35" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>130216</v>
-      </c>
-      <c r="G35" s="39">
+        <v>229263</v>
+      </c>
+      <c r="G35" s="44">
         <f t="shared" ref="G35" ca="1" si="13">F35+F36+F37</f>
-        <v>656585</v>
+        <v>604433</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="40"/>
-      <c r="B36" s="40"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="41"/>
       <c r="C36" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D36" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="E36" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="F36" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>332545</v>
-      </c>
-      <c r="G36" s="39"/>
+        <v>264457</v>
+      </c>
+      <c r="G36" s="44"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D37" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>237</v>
+        <v>161</v>
       </c>
       <c r="E37" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F37" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>193824</v>
-      </c>
-      <c r="G37" s="39"/>
+        <v>110713</v>
+      </c>
+      <c r="G37" s="44"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="40">
+      <c r="A38" s="41">
         <v>13</v>
       </c>
-      <c r="B38" s="40" t="s">
+      <c r="B38" s="41" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="4" t="s">
@@ -2334,66 +2334,66 @@
       </c>
       <c r="D38" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>216</v>
+        <v>287</v>
       </c>
       <c r="E38" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="F38" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>260808</v>
-      </c>
-      <c r="G38" s="39">
+        <v>341902</v>
+      </c>
+      <c r="G38" s="44">
         <f t="shared" ref="G38" ca="1" si="14">F38+F39+F40</f>
-        <v>890774</v>
+        <v>862643</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="40"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D39" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>167</v>
+        <v>281</v>
       </c>
       <c r="E39" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="F39" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>305029</v>
-      </c>
-      <c r="G39" s="39"/>
+        <v>180349</v>
+      </c>
+      <c r="G39" s="44"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="40"/>
-      <c r="B40" s="40"/>
+      <c r="A40" s="41"/>
+      <c r="B40" s="41"/>
       <c r="C40" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>151</v>
+        <v>182</v>
       </c>
       <c r="E40" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F40" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>324937</v>
-      </c>
-      <c r="G40" s="39"/>
+        <v>340392</v>
+      </c>
+      <c r="G40" s="44"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="40">
+      <c r="A41" s="41">
         <v>14</v>
       </c>
-      <c r="B41" s="40" t="s">
+      <c r="B41" s="41" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -2401,50 +2401,50 @@
       </c>
       <c r="D41" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>287</v>
+        <v>101</v>
       </c>
       <c r="E41" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F41" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>276473</v>
-      </c>
-      <c r="G41" s="39">
+        <v>121085</v>
+      </c>
+      <c r="G41" s="44">
         <f t="shared" ref="G41" ca="1" si="15">F41+F42+F43</f>
-        <v>772238</v>
+        <v>578911</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="40"/>
-      <c r="B42" s="40"/>
+      <c r="A42" s="41"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D42" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>100</v>
+        <v>203</v>
       </c>
       <c r="E42" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="F42" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>324348</v>
-      </c>
-      <c r="G42" s="39"/>
+        <v>235986</v>
+      </c>
+      <c r="G42" s="44"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D43" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>234</v>
+        <v>100</v>
       </c>
       <c r="E43" s="3">
         <f t="shared" ca="1" si="1"/>
@@ -2452,15 +2452,15 @@
       </c>
       <c r="F43" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>171417</v>
-      </c>
-      <c r="G43" s="39"/>
+        <v>221840</v>
+      </c>
+      <c r="G43" s="44"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="40">
+      <c r="A44" s="41">
         <v>15</v>
       </c>
-      <c r="B44" s="40" t="s">
+      <c r="B44" s="41" t="s">
         <v>16</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -2468,66 +2468,66 @@
       </c>
       <c r="D44" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>102</v>
+        <v>212</v>
       </c>
       <c r="E44" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="F44" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>108972</v>
-      </c>
-      <c r="G44" s="39">
+        <v>100101</v>
+      </c>
+      <c r="G44" s="44">
         <f t="shared" ref="G44" ca="1" si="16">F44+F45+F46</f>
-        <v>715064</v>
+        <v>436876</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D45" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>97</v>
+        <v>274</v>
       </c>
       <c r="E45" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="F45" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>315248</v>
-      </c>
-      <c r="G45" s="39"/>
+        <v>144893</v>
+      </c>
+      <c r="G45" s="44"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="40"/>
-      <c r="B46" s="40"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="41"/>
       <c r="C46" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D46" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E46" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="F46" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>290844</v>
-      </c>
-      <c r="G46" s="39"/>
+        <v>191882</v>
+      </c>
+      <c r="G46" s="44"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="40">
+      <c r="A47" s="41">
         <v>16</v>
       </c>
-      <c r="B47" s="40" t="s">
+      <c r="B47" s="41" t="s">
         <v>17</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -2535,60 +2535,60 @@
       </c>
       <c r="D47" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>300</v>
+        <v>155</v>
       </c>
       <c r="E47" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="F47" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>233699</v>
-      </c>
-      <c r="G47" s="39">
+        <v>150490</v>
+      </c>
+      <c r="G47" s="44">
         <f t="shared" ref="G47" ca="1" si="17">F47+F48+F49</f>
-        <v>803254</v>
+        <v>677040</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="40"/>
-      <c r="B48" s="40"/>
+      <c r="A48" s="41"/>
+      <c r="B48" s="41"/>
       <c r="C48" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D48" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>179</v>
+        <v>230</v>
       </c>
       <c r="E48" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="F48" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>318363</v>
-      </c>
-      <c r="G48" s="39"/>
+        <v>334344</v>
+      </c>
+      <c r="G48" s="44"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="40"/>
-      <c r="B49" s="40"/>
+      <c r="A49" s="41"/>
+      <c r="B49" s="41"/>
       <c r="C49" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D49" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>265</v>
+        <v>95</v>
       </c>
       <c r="E49" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F49" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>251192</v>
-      </c>
-      <c r="G49" s="39"/>
+        <v>192206</v>
+      </c>
+      <c r="G49" s="44"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="42">
@@ -2602,19 +2602,19 @@
       </c>
       <c r="D50" s="10">
         <f t="shared" ca="1" si="3"/>
-        <v>246</v>
+        <v>219</v>
       </c>
       <c r="E50" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F50" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>267179</v>
-      </c>
-      <c r="G50" s="38">
+        <v>133613</v>
+      </c>
+      <c r="G50" s="45">
         <f t="shared" ref="G50" ca="1" si="18">F50+F51+F52</f>
-        <v>851075</v>
+        <v>683230</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
@@ -2625,17 +2625,17 @@
       </c>
       <c r="D51" s="10">
         <f t="shared" ca="1" si="3"/>
-        <v>82</v>
+        <v>222</v>
       </c>
       <c r="E51" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="F51" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>250891</v>
-      </c>
-      <c r="G51" s="38"/>
+        <v>206900</v>
+      </c>
+      <c r="G51" s="45"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="42"/>
@@ -2645,23 +2645,23 @@
       </c>
       <c r="D52" s="10">
         <f t="shared" ca="1" si="3"/>
-        <v>255</v>
+        <v>287</v>
       </c>
       <c r="E52" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F52" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>333005</v>
-      </c>
-      <c r="G52" s="38"/>
+        <v>342717</v>
+      </c>
+      <c r="G52" s="45"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="40">
+      <c r="A53" s="41">
         <v>18</v>
       </c>
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="41" t="s">
         <v>19</v>
       </c>
       <c r="C53" s="4" t="s">
@@ -2669,66 +2669,66 @@
       </c>
       <c r="D53" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="E53" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F53" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>107068</v>
-      </c>
-      <c r="G53" s="39">
+        <v>133023</v>
+      </c>
+      <c r="G53" s="44">
         <f t="shared" ref="G53" ca="1" si="19">F53+F54+F55</f>
-        <v>689433</v>
+        <v>505028</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="40"/>
-      <c r="B54" s="40"/>
+      <c r="A54" s="41"/>
+      <c r="B54" s="41"/>
       <c r="C54" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D54" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>80</v>
+        <v>298</v>
       </c>
       <c r="E54" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F54" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>276328</v>
-      </c>
-      <c r="G54" s="39"/>
+        <v>175859</v>
+      </c>
+      <c r="G54" s="44"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" s="40"/>
-      <c r="B55" s="40"/>
+      <c r="A55" s="41"/>
+      <c r="B55" s="41"/>
       <c r="C55" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D55" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>225</v>
+        <v>153</v>
       </c>
       <c r="E55" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F55" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>306037</v>
-      </c>
-      <c r="G55" s="39"/>
+        <v>196146</v>
+      </c>
+      <c r="G55" s="44"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A56" s="40">
+      <c r="A56" s="41">
         <v>19</v>
       </c>
-      <c r="B56" s="40" t="s">
+      <c r="B56" s="41" t="s">
         <v>20</v>
       </c>
       <c r="C56" s="4" t="s">
@@ -2736,66 +2736,66 @@
       </c>
       <c r="D56" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>287</v>
+        <v>195</v>
       </c>
       <c r="E56" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F56" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>213747</v>
-      </c>
-      <c r="G56" s="39">
+        <v>215919</v>
+      </c>
+      <c r="G56" s="44">
         <f t="shared" ref="G56" ca="1" si="20">F56+F57+F58</f>
-        <v>622713</v>
+        <v>693245</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A57" s="40"/>
-      <c r="B57" s="40"/>
+      <c r="A57" s="41"/>
+      <c r="B57" s="41"/>
       <c r="C57" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D57" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>191</v>
+        <v>117</v>
       </c>
       <c r="E57" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F57" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>166729</v>
-      </c>
-      <c r="G57" s="39"/>
+        <v>349432</v>
+      </c>
+      <c r="G57" s="44"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A58" s="40"/>
-      <c r="B58" s="40"/>
+      <c r="A58" s="41"/>
+      <c r="B58" s="41"/>
       <c r="C58" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D58" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>188</v>
+        <v>235</v>
       </c>
       <c r="E58" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F58" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>242237</v>
-      </c>
-      <c r="G58" s="39"/>
+        <v>127894</v>
+      </c>
+      <c r="G58" s="44"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" s="40">
+      <c r="A59" s="41">
         <v>20</v>
       </c>
-      <c r="B59" s="40" t="s">
+      <c r="B59" s="41" t="s">
         <v>21</v>
       </c>
       <c r="C59" s="4" t="s">
@@ -2803,100 +2803,80 @@
       </c>
       <c r="D59" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="E59" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F59" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>342349</v>
-      </c>
-      <c r="G59" s="39">
+        <v>227658</v>
+      </c>
+      <c r="G59" s="44">
         <f t="shared" ref="G59" ca="1" si="21">F59+F60+F61</f>
-        <v>637150</v>
+        <v>652035</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A60" s="40"/>
-      <c r="B60" s="40"/>
+      <c r="A60" s="41"/>
+      <c r="B60" s="41"/>
       <c r="C60" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D60" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E60" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F60" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>143742</v>
-      </c>
-      <c r="G60" s="39"/>
+        <v>155088</v>
+      </c>
+      <c r="G60" s="44"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="40"/>
-      <c r="B61" s="40"/>
+      <c r="A61" s="41"/>
+      <c r="B61" s="41"/>
       <c r="C61" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D61" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>164</v>
+        <v>294</v>
       </c>
       <c r="E61" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="F61" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>151059</v>
-      </c>
-      <c r="G61" s="39"/>
+        <v>269289</v>
+      </c>
+      <c r="G61" s="44"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F62" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="G50:G52"/>
+    <mergeCell ref="G53:G55"/>
+    <mergeCell ref="G56:G58"/>
+    <mergeCell ref="G59:G61"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="G47:G49"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="G32:G34"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="G2:G4"/>
     <mergeCell ref="G5:G7"/>
@@ -2909,20 +2889,40 @@
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="B14:B16"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="G32:G34"/>
-    <mergeCell ref="G50:G52"/>
-    <mergeCell ref="G53:G55"/>
-    <mergeCell ref="G56:G58"/>
-    <mergeCell ref="G59:G61"/>
-    <mergeCell ref="G35:G37"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="G41:G43"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="G47:G49"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A14:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2933,8 +2933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76D7D46-21B7-054F-A2A5-55DC0853579C}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2980,23 +2980,23 @@
       </c>
       <c r="C2" s="3">
         <f ca="1">RANDBETWEEN(2000,12000)</f>
-        <v>12000</v>
+        <v>7986</v>
       </c>
       <c r="D2" s="3">
         <f ca="1">RANDBETWEEN(100,1000)</f>
-        <v>906</v>
+        <v>965</v>
       </c>
       <c r="E2" s="6">
         <f ca="1">RANDBETWEEN(100000,350000)</f>
-        <v>328543</v>
+        <v>347286</v>
       </c>
       <c r="F2" s="6">
         <f ca="1">RANDBETWEEN(100000,350000)</f>
-        <v>200875</v>
+        <v>134110</v>
       </c>
       <c r="G2" s="19">
         <f ca="1">RANDBETWEEN(300000,800000)</f>
-        <v>342383</v>
+        <v>778381</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -3008,23 +3008,23 @@
       </c>
       <c r="C3" s="3">
         <f t="shared" ref="C3:C21" ca="1" si="0">RANDBETWEEN(2000,12000)</f>
-        <v>6736</v>
+        <v>7334</v>
       </c>
       <c r="D3" s="3">
         <f t="shared" ref="D3:D21" ca="1" si="1">RANDBETWEEN(100,1000)</f>
-        <v>147</v>
+        <v>454</v>
       </c>
       <c r="E3" s="6">
         <f t="shared" ref="E3:F21" ca="1" si="2">RANDBETWEEN(100000,350000)</f>
-        <v>264378</v>
+        <v>115512</v>
       </c>
       <c r="F3" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>290081</v>
+        <v>335778</v>
       </c>
       <c r="G3" s="19">
         <f t="shared" ref="G3:G21" ca="1" si="3">RANDBETWEEN(300000,800000)</f>
-        <v>581060</v>
+        <v>406012</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -3036,23 +3036,23 @@
       </c>
       <c r="C4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>2855</v>
+        <v>10836</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>622</v>
+        <v>229</v>
       </c>
       <c r="E4" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>110634</v>
+        <v>156392</v>
       </c>
       <c r="F4" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>260394</v>
+        <v>310163</v>
       </c>
       <c r="G4" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>691454</v>
+        <v>313951</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -3064,23 +3064,23 @@
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>10642</v>
+        <v>8744</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>730</v>
+        <v>523</v>
       </c>
       <c r="E5" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>163420</v>
+        <v>305642</v>
       </c>
       <c r="F5" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>324099</v>
+        <v>231914</v>
       </c>
       <c r="G5" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>665228</v>
+        <v>651329</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -3092,23 +3092,23 @@
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5565</v>
+        <v>7688</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>442</v>
+        <v>598</v>
       </c>
       <c r="E6" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>258454</v>
+        <v>129978</v>
       </c>
       <c r="F6" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>145750</v>
+        <v>237804</v>
       </c>
       <c r="G6" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>561189</v>
+        <v>718826</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -3120,23 +3120,23 @@
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>4450</v>
+        <v>10035</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>920</v>
+        <v>609</v>
       </c>
       <c r="E7" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>156847</v>
+        <v>172242</v>
       </c>
       <c r="F7" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>173708</v>
+        <v>252934</v>
       </c>
       <c r="G7" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>340848</v>
+        <v>737536</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -3148,23 +3148,23 @@
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5190</v>
+        <v>4399</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>630</v>
+        <v>475</v>
       </c>
       <c r="E8" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>222964</v>
+        <v>245907</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>189575</v>
+        <v>237227</v>
       </c>
       <c r="G8" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>536384</v>
+        <v>342807</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -3176,23 +3176,23 @@
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8107</v>
+        <v>10154</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>498</v>
+        <v>868</v>
       </c>
       <c r="E9" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>221645</v>
+        <v>157465</v>
       </c>
       <c r="F9" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>333127</v>
+        <v>252665</v>
       </c>
       <c r="G9" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>598508</v>
+        <v>657326</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -3204,23 +3204,23 @@
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>2885</v>
+        <v>5987</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>987</v>
+        <v>525</v>
       </c>
       <c r="E10" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>225035</v>
+        <v>185816</v>
       </c>
       <c r="F10" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>300406</v>
+        <v>190902</v>
       </c>
       <c r="G10" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>453034</v>
+        <v>645970</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -3232,23 +3232,23 @@
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6401</v>
+        <v>9851</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>641</v>
+        <v>915</v>
       </c>
       <c r="E11" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>302440</v>
+        <v>323232</v>
       </c>
       <c r="F11" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>259939</v>
+        <v>143629</v>
       </c>
       <c r="G11" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>496086</v>
+        <v>655144</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -3260,23 +3260,23 @@
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6556</v>
+        <v>11167</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>848</v>
+        <v>148</v>
       </c>
       <c r="E12" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>192592</v>
+        <v>325274</v>
       </c>
       <c r="F12" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>252932</v>
+        <v>194297</v>
       </c>
       <c r="G12" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>471843</v>
+        <v>669141</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -3288,23 +3288,23 @@
       </c>
       <c r="C13" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6100</v>
+        <v>7283</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>158</v>
+        <v>204</v>
       </c>
       <c r="E13" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>284836</v>
+        <v>207342</v>
       </c>
       <c r="F13" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>160564</v>
+        <v>308566</v>
       </c>
       <c r="G13" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>451848</v>
+        <v>531521</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -3316,23 +3316,23 @@
       </c>
       <c r="C14" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5660</v>
+        <v>4000</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>344</v>
+        <v>558</v>
       </c>
       <c r="E14" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>107645</v>
+        <v>154581</v>
       </c>
       <c r="F14" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>137819</v>
+        <v>310130</v>
       </c>
       <c r="G14" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>761172</v>
+        <v>515553</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -3344,23 +3344,23 @@
       </c>
       <c r="C15" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8644</v>
+        <v>6142</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="E15" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>224945</v>
+        <v>110812</v>
       </c>
       <c r="F15" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>265373</v>
+        <v>105989</v>
       </c>
       <c r="G15" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>359961</v>
+        <v>763516</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -3372,23 +3372,23 @@
       </c>
       <c r="C16" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6305</v>
+        <v>7260</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>749</v>
+        <v>110</v>
       </c>
       <c r="E16" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>127023</v>
+        <v>258508</v>
       </c>
       <c r="F16" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>161845</v>
+        <v>215147</v>
       </c>
       <c r="G16" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>632283</v>
+        <v>751475</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -3400,23 +3400,23 @@
       </c>
       <c r="C17" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7916</v>
+        <v>6108</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>937</v>
+        <v>702</v>
       </c>
       <c r="E17" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>220521</v>
+        <v>298003</v>
       </c>
       <c r="F17" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>163970</v>
+        <v>202170</v>
       </c>
       <c r="G17" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>769605</v>
+        <v>735946</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -3428,23 +3428,23 @@
       </c>
       <c r="C18" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>3506</v>
+        <v>10705</v>
       </c>
       <c r="D18" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>483</v>
+        <v>877</v>
       </c>
       <c r="E18" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>206628</v>
+        <v>245447</v>
       </c>
       <c r="F18" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>262350</v>
+        <v>242266</v>
       </c>
       <c r="G18" s="22">
         <f t="shared" ca="1" si="3"/>
-        <v>342713</v>
+        <v>310050</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -3456,23 +3456,23 @@
       </c>
       <c r="C19" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>11554</v>
+        <v>8216</v>
       </c>
       <c r="D19" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>185</v>
+        <v>665</v>
       </c>
       <c r="E19" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>103340</v>
+        <v>162099</v>
       </c>
       <c r="F19" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>328245</v>
+        <v>149358</v>
       </c>
       <c r="G19" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>701073</v>
+        <v>347863</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -3484,23 +3484,23 @@
       </c>
       <c r="C20" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>4250</v>
+        <v>5176</v>
       </c>
       <c r="D20" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>553</v>
+        <v>373</v>
       </c>
       <c r="E20" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>290159</v>
+        <v>118180</v>
       </c>
       <c r="F20" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>308273</v>
+        <v>336567</v>
       </c>
       <c r="G20" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>320779</v>
+        <v>654994</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -3512,23 +3512,23 @@
       </c>
       <c r="C21" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>11685</v>
+        <v>6085</v>
       </c>
       <c r="D21" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>914</v>
+        <v>810</v>
       </c>
       <c r="E21" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>192154</v>
+        <v>241470</v>
       </c>
       <c r="F21" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>116772</v>
+        <v>250258</v>
       </c>
       <c r="G21" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>754795</v>
+        <v>625681</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -3545,7 +3545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CF643C-5C0E-744E-967C-222C017A8BAB}">
   <dimension ref="A1:AE26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
@@ -5791,7 +5791,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B11"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5860,10 +5860,10 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="45">
+      <c r="B2" s="40">
         <v>1122334455</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="38" t="s">
         <v>168</v>
       </c>
       <c r="D2" s="33" t="s">
@@ -5887,16 +5887,16 @@
       <c r="J2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="43" t="s">
+      <c r="K2" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="L2" s="44" t="s">
+      <c r="L2" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="M2" s="45" t="s">
+      <c r="M2" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="N2" s="43" t="s">
+      <c r="N2" s="38" t="s">
         <v>167</v>
       </c>
     </row>
@@ -5904,10 +5904,10 @@
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="45">
+      <c r="B3" s="40">
         <v>1122334455</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="38" t="s">
         <v>275</v>
       </c>
       <c r="D3" s="33" t="s">
@@ -5931,16 +5931,16 @@
       <c r="J3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="M3" s="45" t="s">
+      <c r="M3" s="40" t="s">
         <v>280</v>
       </c>
-      <c r="N3" s="43" t="s">
+      <c r="N3" s="38" t="s">
         <v>289</v>
       </c>
     </row>
@@ -5948,10 +5948,10 @@
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="45">
+      <c r="B4" s="40">
         <v>2233445566</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="38" t="s">
         <v>169</v>
       </c>
       <c r="D4" s="33" t="s">
@@ -5975,16 +5975,16 @@
       <c r="J4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="43" t="s">
+      <c r="K4" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="L4" s="44" t="s">
+      <c r="L4" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="M4" s="45" t="s">
+      <c r="M4" s="40" t="s">
         <v>281</v>
       </c>
-      <c r="N4" s="43" t="s">
+      <c r="N4" s="38" t="s">
         <v>290</v>
       </c>
     </row>
@@ -5992,10 +5992,10 @@
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5" s="40">
         <v>2233445566</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="38" t="s">
         <v>276</v>
       </c>
       <c r="D5" s="33" t="s">
@@ -6019,16 +6019,16 @@
       <c r="J5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="43" t="s">
+      <c r="K5" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="L5" s="44" t="s">
+      <c r="L5" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="M5" s="45" t="s">
+      <c r="M5" s="40" t="s">
         <v>282</v>
       </c>
-      <c r="N5" s="43" t="s">
+      <c r="N5" s="38" t="s">
         <v>291</v>
       </c>
     </row>
@@ -6036,10 +6036,10 @@
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="45">
+      <c r="B6" s="40">
         <v>3344556677</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="38" t="s">
         <v>170</v>
       </c>
       <c r="D6" s="33" t="s">
@@ -6063,16 +6063,16 @@
       <c r="J6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="43" t="s">
+      <c r="K6" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="L6" s="44" t="s">
+      <c r="L6" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="M6" s="45" t="s">
+      <c r="M6" s="40" t="s">
         <v>283</v>
       </c>
-      <c r="N6" s="43" t="s">
+      <c r="N6" s="38" t="s">
         <v>292</v>
       </c>
     </row>
@@ -6080,10 +6080,10 @@
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="45">
+      <c r="B7" s="40">
         <v>3344556677</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="38" t="s">
         <v>277</v>
       </c>
       <c r="D7" s="33" t="s">
@@ -6107,16 +6107,16 @@
       <c r="J7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="43" t="s">
+      <c r="K7" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="L7" s="44" t="s">
+      <c r="L7" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="M7" s="45" t="s">
+      <c r="M7" s="40" t="s">
         <v>284</v>
       </c>
-      <c r="N7" s="43" t="s">
+      <c r="N7" s="38" t="s">
         <v>293</v>
       </c>
     </row>
@@ -6124,10 +6124,10 @@
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="45">
+      <c r="B8" s="40">
         <v>4455667788</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="38" t="s">
         <v>171</v>
       </c>
       <c r="D8" s="33" t="s">
@@ -6151,16 +6151,16 @@
       <c r="J8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="43" t="s">
+      <c r="K8" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="L8" s="44" t="s">
+      <c r="L8" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="M8" s="45" t="s">
+      <c r="M8" s="40" t="s">
         <v>285</v>
       </c>
-      <c r="N8" s="43" t="s">
+      <c r="N8" s="38" t="s">
         <v>294</v>
       </c>
     </row>
@@ -6168,10 +6168,10 @@
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="45">
+      <c r="B9" s="40">
         <v>4455667788</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="38" t="s">
         <v>278</v>
       </c>
       <c r="D9" s="33" t="s">
@@ -6195,16 +6195,16 @@
       <c r="J9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="43" t="s">
+      <c r="K9" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="L9" s="44" t="s">
+      <c r="L9" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="M9" s="45" t="s">
+      <c r="M9" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="N9" s="43" t="s">
+      <c r="N9" s="38" t="s">
         <v>295</v>
       </c>
     </row>
@@ -6212,10 +6212,10 @@
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="45">
+      <c r="B10" s="40">
         <v>5566778899</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="38" t="s">
         <v>172</v>
       </c>
       <c r="D10" s="33" t="s">
@@ -6239,16 +6239,16 @@
       <c r="J10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="43" t="s">
+      <c r="K10" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="L10" s="44" t="s">
+      <c r="L10" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="M10" s="45" t="s">
+      <c r="M10" s="40" t="s">
         <v>287</v>
       </c>
-      <c r="N10" s="43" t="s">
+      <c r="N10" s="38" t="s">
         <v>296</v>
       </c>
     </row>
@@ -6256,10 +6256,10 @@
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="45">
+      <c r="B11" s="40">
         <v>5566778899</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="38" t="s">
         <v>279</v>
       </c>
       <c r="D11" s="33" t="s">
@@ -6283,16 +6283,16 @@
       <c r="J11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="43" t="s">
+      <c r="K11" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="L11" s="44" t="s">
+      <c r="L11" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="M11" s="45" t="s">
+      <c r="M11" s="40" t="s">
         <v>288</v>
       </c>
-      <c r="N11" s="43" t="s">
+      <c r="N11" s="38" t="s">
         <v>297</v>
       </c>
     </row>

</xml_diff>